<commit_message>
sync for file widget dev
</commit_message>
<xml_diff>
--- a/resources/5GNR_default_vals.xlsx
+++ b/resources/5GNR_default_vals.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2653EA-BA99-4B4B-ADFB-F05B02DEFA30}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -34,14 +33,14 @@
     <t>Attenuation(dBm)</t>
   </si>
   <si>
-    <t>C:\\R_S\\Instr\\user\\NR5G\\AllocationFiles\\DL\\Gen4_Malliv31\\Ant0\\64QAM_cellld1_papr11_74.allocation</t>
+    <t>C:\\R_S\\Instr\\user\\NR5G\\AllocationFiles\\DL\\64QAM_cellId1_papr11_74.allocation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,27 +417,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.42578125" customWidth="1"/>
     <col min="2" max="2" width="109.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -446,7 +445,7 @@
         <v>37.40034</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -454,7 +453,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -462,7 +461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
5GNR mode, fixed the synchronization issue with the EVM measurement
</commit_message>
<xml_diff>
--- a/resources/5GNR_default_vals.xlsx
+++ b/resources/5GNR_default_vals.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Allocation File</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>QAM PDSCH</t>
   </si>
@@ -33,7 +30,7 @@
     <t>Attenuation(dBm)</t>
   </si>
   <si>
-    <t>C:\\R_S\\Instr\\user\\NR5G\\AllocationFiles\\DL\\64QAM_cellId1_papr11_74.allocation</t>
+    <t>Number Carriers</t>
   </si>
 </sst>
 </file>
@@ -428,7 +425,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -439,15 +436,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2">
-        <v>37.40034</v>
+        <v>37.394039999999997</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4">
         <v>10</v>
@@ -455,15 +452,15 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1">
       <c r="A4" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="6">
         <v>64</v>

</xml_diff>